<commit_message>
improved database creation notebook
</commit_message>
<xml_diff>
--- a/data/Inventory_Data.xlsx
+++ b/data/Inventory_Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70322C5-0791-486F-B485-6457F9360FF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4EDFA2-4D4A-4DBA-82ED-407F56F4523E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11717" windowHeight="3454" tabRatio="850" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11717" windowHeight="3454" tabRatio="850" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta_Data" sheetId="4" r:id="rId1"/>
@@ -7339,7 +7339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3241006-3FA7-4340-B546-FAB8FC6089D1}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
@@ -10049,7 +10049,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -12267,7 +12267,7 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -12517,11 +12517,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DAD81A-466E-4B0E-B937-7E6ADDD1B384}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -13115,16 +13115,19 @@
       <c r="I16" s="93"/>
       <c r="L16" s="93"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="9:12" x14ac:dyDescent="0.4">
       <c r="I17" s="93"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.4">
-      <c r="I18" s="93"/>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="9:12" x14ac:dyDescent="0.4">
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="89"/>
+    </row>
+    <row r="21" spans="9:12" x14ac:dyDescent="0.4">
       <c r="I21" s="98"/>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="9:12" x14ac:dyDescent="0.4">
       <c r="I22" s="98"/>
     </row>
   </sheetData>

</xml_diff>